<commit_message>
#640 divided by 김미경
</commit_message>
<xml_diff>
--- a/sub/640/en-640-suicidal-impulse.xlsx
+++ b/sub/640/en-640-suicidal-impulse.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Softmirage\Dropbox\YouTube Translation Project\02_Translation\02_Complete\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="15" windowWidth="28500" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="22" r:id="rId1"/>
+    <sheet name="mk" sheetId="24" r:id="rId1"/>
+    <sheet name="original" sheetId="22" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="687">
   <si>
     <t>Q: I have sensitive nerves and insomnia, that disorder, because of PMS, I spend like one third of a month depressed, demotivated and tiredness, and mood swing, negative emotion, decline in concentration, irritation, anger and such, in the case of severe stress, there were times when I had an urge to commit suicide.</t>
   </si>
@@ -1734,13 +1730,378 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=GpJ0gq-TlXE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">저는 신경이 예민해서 불면증이 있고, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">그 병 생리증후군 때문에 한 달에 삼분에 이정도가 우울하고 무기력하고 피로감, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I suffer from PMS for a third of the month with depression, lethargy, fatigue, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">그리고 감정의 기복, 부정적 감정, 집중력 저하, 짜증, 분노 등등을 느끼며, </t>
+  </si>
+  <si>
+    <t>mood swings, declined concentration, irritation, anger, and so on.</t>
+  </si>
+  <si>
+    <t>스트레스가 심할 경우 자살충동을 느낀 적도 있습니다.</t>
+  </si>
+  <si>
+    <t>안 죽으면 되지.어떡하긴.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">예를 들어 어떤 가게를 지나가다가 아주 비싼 물건이 있는데 살라니 돈은 없고, </t>
+  </si>
+  <si>
+    <t>Let's say you pass by a shop, and seeing an expensive item,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이래 딱 보고 훔쳐 가버리고 싶은 충동이 일어날 때 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> you feel the impulse to steal it.</t>
+  </si>
+  <si>
+    <t>어떻게 해야 돼? 훔쳐 버려야 돼? 충동 일어나더라도 안 훔쳐야 돼?</t>
+  </si>
+  <si>
+    <t>어떤 외간 남자 지나가는데 잘 생겼고</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cute guy walks by, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 마 확 가서 껴안아주고 뽀뽀 해주고 싶은데, 충동 일어나는데 </t>
+  </si>
+  <si>
+    <t>and you feel the impulse to hug and kiss him.</t>
+  </si>
+  <si>
+    <t>그래도 자제 해야 돼? 하고 싶다고 해버려야 돼?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are. </t>
+  </si>
+  <si>
+    <t>But we control ourselves as it will be a loss for us not to.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">괜히 남 남자 껴안았다가 망신 살고, 물건 하나 훔쳤다고 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We'll get humiliated by hugging a stranger. </t>
+  </si>
+  <si>
+    <t>도둑놈 잡혀서 감옥 가서 살고.</t>
+  </si>
+  <si>
+    <t>We'll end up in jail for stealing something.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">신문 봐요 안봐요? 안 봐요? </t>
+  </si>
+  <si>
+    <t>Have you seen today's news?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">오늘 신문 보니까 소위 세계은행 IMF 총재가 그 호텔 청소하는 여자를 방에 끌고 들어가, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The head of IMF attempted to rape a hotel maid.</t>
+  </si>
+  <si>
+    <t>방에 청소하러 들어왔는데, 그걸 그냥 강제로 성폭행 하려다가 안됐다.</t>
+  </si>
+  <si>
+    <t>병원에 진료를 좀 더 받고 전문의사의 처방을 받으면서,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get treated by a specialist doctor at the hospital. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 그렇다고 완치 된다는 얘긴 아니에요.</t>
+  </si>
+  <si>
+    <t>But that won't necessarily cure you completely.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">전문의사의 진료를 좀 받으면서 지금 잠이 잘 안 와요? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sleeping well? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">약 먹어야 자요? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you need sleeping pills? </t>
+  </si>
+  <si>
+    <t>그럼 좀 심한 상태예요.</t>
+  </si>
+  <si>
+    <t>Then that's a bit severe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">전문의의 진료를 받아야지 </t>
+  </si>
+  <si>
+    <t>You should follow the doctor's advice</t>
+  </si>
+  <si>
+    <t>혼자 생각해서 진료도 안 받고,  내 맘대로 하면 안돼요.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and not try to treat it on your own.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그 때 생각을 너무 ‘안 죽어야 된다.’ 각오를 하지 말고, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">At that moment, don't focus too much on thinking "I shouldn't die." </t>
+  </si>
+  <si>
+    <t>그 때 생각을 바꾸면 되요.</t>
+  </si>
+  <si>
+    <t>Think of something else.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어떤 사람이 죽을라고 산에 가서 목매 죽을라고 </t>
+  </si>
+  <si>
+    <t>A man went up a mountain to hang himself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">끈을 매가 목을 딱 걸려고 할 때 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> He had a noose tied around his neck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">할때도 고 순간이지 지나면 괜찮고, </t>
+  </si>
+  <si>
+    <t>어디 가서 백화점가서 좋은 물건 보고 훔치고 싶을 때,</t>
+  </si>
+  <si>
+    <t>누가 자살할라고 약을 딱 가지고, 인제 사람 없는데 저 산에 가서 약을 먹고 죽을라고 딱 준비하고 있는데,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A man went up a mountain to kill himself. As he was about to take his pills, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 누가 사람이 지나오는 거예요.</t>
+  </si>
+  <si>
+    <t>somebody walked by.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그러니까 ‘저 사람 지나가면 한다.’ 이래가지고 기다렸다가 그 사람 지나가고 </t>
+  </si>
+  <si>
+    <t>So he waited until that person passed,</t>
+  </si>
+  <si>
+    <t>또 약을 먹을 라니까 저기 또 사람이 오는 거예요.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> but then another person walked by.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그 사람이 지나가고 인제 아무도 없어가지고 약을 딱 입에 댈라 하는데 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The person passed by, so he attempted to take the pills. </t>
+  </si>
+  <si>
+    <t>저 앞에서 자전거를 타고 오는 거예요.</t>
+  </si>
+  <si>
+    <t>But then came a bicycle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">아이고 먹을까 말까 먹을까 말까 멀리 떨어져 있었는데, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darn it, should I take it or not. </t>
+  </si>
+  <si>
+    <t>그래서 자전거니까 빨리 오잖아. 그죠?</t>
+  </si>
+  <si>
+    <t>I'll wait, the bicycle should pass by fast enough', he thought.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 그래서 저 사람만 지나가면 먹어야지.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이 사람이 약간 고개 약간 고갯길에 없는데 올라가서 앉아 있었는데, </t>
+  </si>
+  <si>
+    <t>But then this person gets off his bicycle</t>
+  </si>
+  <si>
+    <t>이 사람 자전거 타고 오다가 자전거가 고개를 못 올라오니까 내려가 걸어 오는 거예요 자전거를 타고.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and starts walking as he can't ride it uphill.</t>
+  </si>
+  <si>
+    <t>그래서 결국 자살 못하고, 약병 들고 왔다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고 순간적인 충동을 이 사람이 원래 평소에 나쁜 행동을 하거나 그런 게 아니더라도 </t>
+  </si>
+  <si>
+    <t>Bad consequences follow</t>
+  </si>
+  <si>
+    <t>어느 순간적인 충동을 자제를 못하면, 인자 그런 큰 손실을 보게 된다. 이런 얘기에요.</t>
+  </si>
+  <si>
+    <t>when a person can't control these momentary impulses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">힘들 때는 되게 힘들고, 근데 약으로 버티고, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are difficult times, but I rely on my medicine. </t>
+  </si>
+  <si>
+    <t>또 괜찮을 때는 잘 지낼 때는 몇 일 괜찮다가 한달에 거의..</t>
+  </si>
+  <si>
+    <t>When I'm okay, I'm fine for a few days…</t>
+  </si>
+  <si>
+    <t>음 그래 혼자서. 둘이 살다가 순간적인 충동에 의해서 죽어 버리면 엄마가 어떨까?</t>
+  </si>
+  <si>
+    <t>여기 절에 법문 들으러 오던지, 와서 봉사를 하던지,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Come to this temple to attend dharma talks, do volunteer work, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 안 그러면 직장동료들하고 수다를 떨던지, 쓸데 없는 수다를 떨던지.</t>
+  </si>
+  <si>
+    <t>or start chatting with your colleagues.</t>
+  </si>
+  <si>
+    <t>여기 정토회 오시면 저 두북이라고 해서 여기 시골에 있는데 가면,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have a Jungto farm out in the countryside </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 풀 뽑을 일도 많고, 밭 맬 일도 많고, 굉장히 많거든요.</t>
+  </si>
+  <si>
+    <t>where we work to remove weeds, till the soil, and lots more.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그런데 가서 하루 종일 일을 해가지고 저녁이 되면, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can work all day there </t>
+  </si>
+  <si>
+    <t>완전히 몸이 피곤해가 몸이 떡이 되도록 이렇게 해가.</t>
+  </si>
+  <si>
+    <t>and completely exhaust yourself,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이런 식으로 육체노동을 많이 하고, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you do lots of physical labor, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">생각은 가능하면 적게 하고, 그래서 피곤해서 잠을 푹 자고, </t>
+  </si>
+  <si>
+    <t>you'll think less and sleep better.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">무슨 생각 들면 고개를 들고 흔들어 버리고, 가서 목욕을 해버리고, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shake it off, take a bath, </t>
+  </si>
+  <si>
+    <t>뭐 밖에 가서 걷고 뛰고, 이렇게 자꾸 생각에 빠지지 마란 말이야.</t>
+  </si>
+  <si>
+    <t>go walk it off, and don't dwell in your head.</t>
+  </si>
+  <si>
+    <t>이렇게 뭐랄까.희화 해버려라.</t>
+  </si>
+  <si>
+    <t>Think lightly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Don't give meaning to every little thing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">아무리 좋은 남자가 있고, 따라 다니고 죽겠다고 해도, </t>
+  </si>
+  <si>
+    <t>And even if you meet a great guy and he begs you to marry him,</t>
+  </si>
+  <si>
+    <t>지금 결혼하면 안돼요.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> don't get married now.</t>
+  </si>
+  <si>
+    <t>지금 결혼하면 안되고,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You shouldn't get married just yet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  결혼 하더라도 괜찮은데, 애기를 낳으면 절대로 지금은 안돼요.</t>
+  </si>
+  <si>
+    <t>But if you do, don't have a baby right now.</t>
+  </si>
+  <si>
+    <t>자살 충동</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Suicidal impulse</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <r>
+      <t>자막이 너무 길어서 김미경 보살님이 자른 버전입</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="굴림"/>
+        <charset val="129"/>
+      </rPr>
+      <t>니다.</t>
+    </r>
+    <phoneticPr fontId="15"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -1830,6 +2191,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.8"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="굴림"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1839,7 +2249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1888,15 +2298,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1931,17 +2358,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1949,16 +2373,66 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2251,22 +2725,1256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C139"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.33203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" style="21" customWidth="1"/>
+    <col min="2" max="3" width="29.6640625" style="26" customWidth="1"/>
+    <col min="4" max="16384" width="7.33203125" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="24" customFormat="1" ht="15">
+      <c r="A1" s="21">
+        <v>640</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="30" customFormat="1" ht="11">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" customHeight="1">
+      <c r="A5" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="41">
+      <c r="B6" s="31" t="s">
+        <v>571</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="33">
+      <c r="B7" s="31" t="s">
+        <v>573</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29">
+      <c r="B8" s="31" t="s">
+        <v>575</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17">
+      <c r="B9" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="13" customHeight="1">
+      <c r="A10" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>576</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29">
+      <c r="A11" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="71" customHeight="1">
+      <c r="A12" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>577</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="71" customHeight="1">
+      <c r="B13" s="31" t="s">
+        <v>579</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29">
+      <c r="B14" s="31" t="s">
+        <v>581</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17">
+      <c r="A15" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="63" customHeight="1">
+      <c r="A16" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>582</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="63" customHeight="1">
+      <c r="B17" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="32.25" customHeight="1">
+      <c r="B18" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17">
+      <c r="A19" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="41">
+      <c r="A20" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17">
+      <c r="A21" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" customHeight="1">
+      <c r="A22" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29">
+      <c r="B23" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17">
+      <c r="A24" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.5" customHeight="1">
+      <c r="A25" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29">
+      <c r="B26" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="29">
+      <c r="B27" s="33" t="s">
+        <v>589</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="29">
+      <c r="B28" s="33" t="s">
+        <v>591</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="98.5" customHeight="1">
+      <c r="B29" s="31" t="s">
+        <v>593</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="98.5" customHeight="1">
+      <c r="B30" s="31" t="s">
+        <v>595</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="76.5" customHeight="1">
+      <c r="B31" s="31" t="s">
+        <v>597</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17">
+      <c r="B32" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="29">
+      <c r="B33" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17">
+      <c r="B34" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17">
+      <c r="A35" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="22">
+      <c r="A36" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29">
+      <c r="B37" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="29">
+      <c r="B38" s="33" t="s">
+        <v>598</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29">
+      <c r="B39" s="33" t="s">
+        <v>600</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="29">
+      <c r="B40" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="22">
+      <c r="B41" s="33" t="s">
+        <v>602</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17">
+      <c r="B42" s="33" t="s">
+        <v>604</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17">
+      <c r="B43" s="33" t="s">
+        <v>606</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17">
+      <c r="B44" s="33" t="s">
+        <v>608</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="22">
+      <c r="B45" s="33" t="s">
+        <v>610</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="29">
+      <c r="B46" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="33">
+      <c r="B47" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17">
+      <c r="A48" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="29">
+      <c r="A49" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>612</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17">
+      <c r="B50" s="33" t="s">
+        <v>614</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17">
+      <c r="B51" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="29">
+      <c r="B52" s="33" t="s">
+        <v>616</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17">
+      <c r="B53" s="33" t="s">
+        <v>618</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="29">
+      <c r="B54" s="33" t="s">
+        <v>389</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="29">
+      <c r="B55" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="29">
+      <c r="B56" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="41">
+      <c r="B57" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="29">
+      <c r="B58" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="29">
+      <c r="B59" s="33" t="s">
+        <v>621</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="29">
+      <c r="B60" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="29">
+      <c r="B61" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="29">
+      <c r="B62" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="29">
+      <c r="B63" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="41">
+      <c r="B64" s="33" t="s">
+        <v>622</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="17">
+      <c r="B65" s="33" t="s">
+        <v>624</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="33">
+      <c r="B66" s="33" t="s">
+        <v>626</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="22">
+      <c r="B67" s="33" t="s">
+        <v>628</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="22">
+      <c r="B68" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="29">
+      <c r="B69" s="33" t="s">
+        <v>630</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="22">
+      <c r="B70" s="33" t="s">
+        <v>632</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="39" customHeight="1">
+      <c r="B71" s="33" t="s">
+        <v>634</v>
+      </c>
+      <c r="C71" s="35" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="39" customHeight="1">
+      <c r="B72" s="33" t="s">
+        <v>636</v>
+      </c>
+      <c r="C72" s="34" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="22">
+      <c r="B73" s="33" t="s">
+        <v>638</v>
+      </c>
+      <c r="C73" s="34" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="29">
+      <c r="B74" s="33" t="s">
+        <v>639</v>
+      </c>
+      <c r="C74" s="32" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="33">
+      <c r="B75" s="33" t="s">
+        <v>641</v>
+      </c>
+      <c r="C75" s="32" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="29">
+      <c r="B76" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="29">
+      <c r="B77" s="33" t="s">
+        <v>643</v>
+      </c>
+      <c r="C77" s="32" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="17">
+      <c r="B78" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" s="32" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="17">
+      <c r="B79" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" ht="29">
+      <c r="B80" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="32" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="41">
+      <c r="B81" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="32" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="41">
+      <c r="B82" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="32" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="33">
+      <c r="B83" s="33" t="s">
+        <v>644</v>
+      </c>
+      <c r="C83" s="32" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="33">
+      <c r="B84" s="33" t="s">
+        <v>646</v>
+      </c>
+      <c r="C84" s="36" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="22">
+      <c r="B85" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C85" s="32" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="22">
+      <c r="B86" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86" s="32" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17">
+      <c r="B87" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="32" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17">
+      <c r="A88" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B88" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="C88" s="32" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="22">
+      <c r="A89" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B89" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" s="32" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="29">
+      <c r="A90" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="C90" s="32" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="17">
+      <c r="A91" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B91" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="C91" s="32" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="29">
+      <c r="A92" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B92" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="C92" s="32" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="22">
+      <c r="B93" s="33" t="s">
+        <v>650</v>
+      </c>
+      <c r="C93" s="36" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="22">
+      <c r="A94" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="C94" s="32" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="17">
+      <c r="A95" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B95" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="C95" s="32" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="47.5" customHeight="1">
+      <c r="A96" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B96" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="C96" s="34" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17">
+      <c r="A97" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B97" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="C97" s="32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="29">
+      <c r="A98" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="C98" s="32" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="29">
+      <c r="A99" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B99" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="C99" s="32" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="22">
+      <c r="A100" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B100" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="C100" s="32" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="29">
+      <c r="B101" s="33" t="s">
+        <v>653</v>
+      </c>
+      <c r="C101" s="32" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="22">
+      <c r="B102" s="33" t="s">
+        <v>655</v>
+      </c>
+      <c r="C102" s="32" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="29">
+      <c r="B103" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" s="32" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17">
+      <c r="B104" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C104" s="32" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="22">
+      <c r="A105" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B105" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="C105" s="32" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="29">
+      <c r="A106" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B106" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="C106" s="32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="29">
+      <c r="B107" s="33" t="s">
+        <v>657</v>
+      </c>
+      <c r="C107" s="32" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="29">
+      <c r="B108" s="33" t="s">
+        <v>659</v>
+      </c>
+      <c r="C108" s="32" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="22">
+      <c r="B109" s="33" t="s">
+        <v>661</v>
+      </c>
+      <c r="C109" s="32" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="22">
+      <c r="B110" s="33" t="s">
+        <v>663</v>
+      </c>
+      <c r="C110" s="32" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="29">
+      <c r="B111" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C111" s="32" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17">
+      <c r="B112" s="33" t="s">
+        <v>665</v>
+      </c>
+      <c r="C112" s="32" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="22">
+      <c r="B113" s="33" t="s">
+        <v>667</v>
+      </c>
+      <c r="C113" s="32" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="41">
+      <c r="B114" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="C114" s="32" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" ht="33">
+      <c r="B115" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" s="32" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" ht="22">
+      <c r="B116" s="33" t="s">
+        <v>669</v>
+      </c>
+      <c r="C116" s="32" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" ht="29">
+      <c r="B117" s="33" t="s">
+        <v>671</v>
+      </c>
+      <c r="C117" s="32" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="26" customHeight="1">
+      <c r="B118" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C118" s="37" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B119" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C119" s="34" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" ht="31" customHeight="1">
+      <c r="B120" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C120" s="34" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B121" s="33" t="s">
+        <v>673</v>
+      </c>
+      <c r="C121" s="34" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B122" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C122" s="34" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" ht="22">
+      <c r="B123" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C123" s="32" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" ht="29">
+      <c r="B124" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C124" s="32" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" ht="17">
+      <c r="B125" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C125" s="32" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" ht="22">
+      <c r="B126" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C126" s="32" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" ht="29">
+      <c r="B127" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C127" s="32" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" ht="17">
+      <c r="B128" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C128" s="32" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="17">
+      <c r="A129" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B129" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="C129" s="32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="17">
+      <c r="A130" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B130" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="C130" s="32" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="29">
+      <c r="B131" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C131" s="32" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15">
+      <c r="B132" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C132" s="37" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="29">
+      <c r="B133" s="33" t="s">
+        <v>676</v>
+      </c>
+      <c r="C133" s="32" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="17">
+      <c r="B134" s="33" t="s">
+        <v>678</v>
+      </c>
+      <c r="C134" s="32" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="17">
+      <c r="B135" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C135" s="32" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="17">
+      <c r="B136" s="33" t="s">
+        <v>680</v>
+      </c>
+      <c r="C136" s="32" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="29">
+      <c r="B137" s="33" t="s">
+        <v>682</v>
+      </c>
+      <c r="C137" s="32" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="17">
+      <c r="B138" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C138" s="32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="29">
+      <c r="B139" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C139" s="32" t="s">
+        <v>568</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="15"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="4" customWidth="1"/>
-    <col min="2" max="3" width="35.7109375" style="7" customWidth="1"/>
-    <col min="4" max="7" width="35.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="49.28515625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="3.83203125" style="4" customWidth="1"/>
+    <col min="2" max="3" width="35.6640625" style="7" customWidth="1"/>
+    <col min="4" max="7" width="35.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="49.33203125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="4">
         <v>640</v>
       </c>
@@ -2281,7 +3989,7 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>569</v>
       </c>
       <c r="E2" s="10"/>
@@ -2289,7 +3997,7 @@
     <row r="3" spans="1:7">
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>167</v>
@@ -2310,14 +4018,14 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="150.75" thickBot="1">
+    <row r="5" spans="1:7" ht="136" thickBot="1">
       <c r="A5" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>486</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -2333,9 +4041,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75.75" thickBot="1">
-      <c r="B6" s="14"/>
-      <c r="C6" s="16" t="s">
+    <row r="6" spans="1:7" ht="76" thickBot="1">
+      <c r="B6" s="20"/>
+      <c r="C6" s="14" t="s">
         <v>487</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -2345,9 +4053,9 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="45.75" thickBot="1">
-      <c r="B7" s="14"/>
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="1:7" ht="31" thickBot="1">
+      <c r="B7" s="20"/>
+      <c r="C7" s="14" t="s">
         <v>488</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -2361,11 +4069,11 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>489</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -2381,9 +4089,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="B9" s="8"/>
-      <c r="C9" s="17"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -2396,10 +4104,10 @@
       <c r="B10" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>490</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="19" t="s">
         <v>363</v>
       </c>
       <c r="E10" s="10" t="s">
@@ -2412,12 +4120,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1">
       <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="10" t="s">
         <v>5</v>
       </c>
@@ -2428,22 +4136,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="B12" s="8"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75" thickBot="1">
+    <row r="13" spans="1:7" ht="31" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>491</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -2459,22 +4167,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="B14" s="8"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="135.75" thickBot="1">
+    <row r="15" spans="1:7" ht="106" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>492</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -2490,9 +4198,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30.75" thickBot="1">
-      <c r="B16" s="14"/>
-      <c r="C16" s="16" t="s">
+    <row r="16" spans="1:7" ht="31" thickBot="1">
+      <c r="B16" s="20"/>
+      <c r="C16" s="14" t="s">
         <v>493</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -2506,22 +4214,22 @@
       </c>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+    <row r="17" spans="1:7" ht="16" thickBot="1">
       <c r="B17" s="8"/>
-      <c r="C17" s="17"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>494</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -2537,9 +4245,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="B19" s="8"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -2549,53 +4257,53 @@
       <c r="A20" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="14" t="s">
         <v>495</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B21" s="14"/>
-      <c r="C21" s="16" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="14" t="s">
         <v>496</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" thickBot="1">
       <c r="B22" s="8"/>
-      <c r="C22" s="17"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:7" ht="16" thickBot="1">
       <c r="A23" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="14" t="s">
         <v>280</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -2611,22 +4319,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="B24" s="8"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" ht="45.75" thickBot="1">
+    <row r="25" spans="1:7" ht="46" thickBot="1">
       <c r="A25" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>281</v>
       </c>
       <c r="D25" s="10" t="s">
@@ -2642,22 +4350,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="B26" s="8"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="14" t="s">
         <v>280</v>
       </c>
       <c r="D27" s="10" t="s">
@@ -2673,25 +4381,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+    <row r="28" spans="1:7" ht="16" thickBot="1">
       <c r="B28" s="8"/>
-      <c r="C28" s="17"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
+    <row r="29" spans="1:7" ht="16" thickBot="1">
       <c r="A29" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="19" t="s">
         <v>370</v>
       </c>
       <c r="E29" s="10" t="s">
@@ -2704,14 +4412,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30.75" thickBot="1">
+    <row r="30" spans="1:7" ht="31" thickBot="1">
       <c r="B30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="14" t="s">
         <v>498</v>
       </c>
-      <c r="D30" s="15"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="10" t="s">
         <v>283</v>
       </c>
@@ -2722,22 +4430,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1">
+    <row r="31" spans="1:7" ht="16" thickBot="1">
       <c r="B31" s="8"/>
-      <c r="C31" s="17"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1">
+    <row r="32" spans="1:7" ht="16" thickBot="1">
       <c r="A32" s="4" t="s">
         <v>180</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="14" t="s">
         <v>284</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -2753,9 +4461,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+    <row r="33" spans="1:7" ht="16" thickBot="1">
       <c r="B33" s="8"/>
-      <c r="C33" s="17"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -2768,10 +4476,10 @@
       <c r="B34" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="19" t="s">
         <v>371</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -2784,12 +4492,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45.75" thickBot="1">
+    <row r="35" spans="1:7" ht="31" thickBot="1">
       <c r="B35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="15"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="10" t="s">
         <v>210</v>
       </c>
@@ -2800,11 +4508,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="60.75" thickBot="1">
+    <row r="36" spans="1:7" ht="46" thickBot="1">
       <c r="B36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="14" t="s">
         <v>500</v>
       </c>
       <c r="D36" s="10" t="s">
@@ -2820,43 +4528,43 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="41.25" thickBot="1">
-      <c r="B37" s="14" t="s">
+    <row r="37" spans="1:7" ht="31" thickBot="1">
+      <c r="B37" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="14" t="s">
         <v>501</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="76.5" customHeight="1" thickBot="1">
-      <c r="B38" s="14"/>
-      <c r="C38" s="16" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="14" t="s">
         <v>502</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="1:7" ht="30.75" thickBot="1">
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="1:7" ht="31" thickBot="1">
       <c r="B39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="14" t="s">
         <v>503</v>
       </c>
       <c r="D39" s="10" t="s">
@@ -2872,11 +4580,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="45.75" thickBot="1">
+    <row r="40" spans="1:7" ht="46" thickBot="1">
       <c r="B40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="14" t="s">
         <v>504</v>
       </c>
       <c r="D40" s="10" t="s">
@@ -2892,11 +4600,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1">
+    <row r="41" spans="1:7" ht="16" thickBot="1">
       <c r="B41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="10" t="s">
@@ -2912,22 +4620,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+    <row r="42" spans="1:7" ht="16" thickBot="1">
       <c r="B42" s="8"/>
-      <c r="C42" s="17"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7" ht="30.75" thickBot="1">
+    <row r="43" spans="1:7" ht="31" thickBot="1">
       <c r="A43" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="14" t="s">
         <v>287</v>
       </c>
       <c r="D43" s="10" t="s">
@@ -2943,22 +4651,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+    <row r="44" spans="1:7" ht="16" thickBot="1">
       <c r="B44" s="8"/>
-      <c r="C44" s="17"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" ht="30.75" thickBot="1">
+    <row r="45" spans="1:7" ht="31" thickBot="1">
       <c r="A45" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="14" t="s">
         <v>505</v>
       </c>
       <c r="D45" s="10" t="s">
@@ -2974,11 +4682,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="45.75" thickBot="1">
+    <row r="46" spans="1:7" ht="31" thickBot="1">
       <c r="B46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="14" t="s">
         <v>506</v>
       </c>
       <c r="D46" s="10" t="s">
@@ -2994,11 +4702,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="60.75" thickBot="1">
+    <row r="47" spans="1:7" ht="61" thickBot="1">
       <c r="B47" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="14" t="s">
         <v>507</v>
       </c>
       <c r="D47" s="10" t="s">
@@ -3014,11 +4722,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30.75" thickBot="1">
+    <row r="48" spans="1:7" ht="31" thickBot="1">
       <c r="B48" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="14" t="s">
         <v>291</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -3034,11 +4742,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="75.75" thickBot="1">
+    <row r="49" spans="1:7" ht="76" thickBot="1">
       <c r="B49" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="14" t="s">
         <v>508</v>
       </c>
       <c r="D49" s="10" t="s">
@@ -3054,11 +4762,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="60.75" thickBot="1">
+    <row r="50" spans="1:7" ht="61" thickBot="1">
       <c r="B50" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="14" t="s">
         <v>509</v>
       </c>
       <c r="D50" s="10" t="s">
@@ -3074,11 +4782,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30.75" thickBot="1">
+    <row r="51" spans="1:7" ht="31" thickBot="1">
       <c r="B51" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="14" t="s">
         <v>510</v>
       </c>
       <c r="D51" s="10" t="s">
@@ -3094,11 +4802,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="45.75" thickBot="1">
+    <row r="52" spans="1:7" ht="46" thickBot="1">
       <c r="B52" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="14" t="s">
         <v>383</v>
       </c>
       <c r="D52" s="10" t="s">
@@ -3114,22 +4822,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1">
+    <row r="53" spans="1:7" ht="16" thickBot="1">
       <c r="B53" s="8"/>
-      <c r="C53" s="17"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1">
+    <row r="54" spans="1:7" ht="16" thickBot="1">
       <c r="A54" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="14" t="s">
         <v>511</v>
       </c>
       <c r="D54" s="10" t="s">
@@ -3145,22 +4853,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1">
+    <row r="55" spans="1:7" ht="16" thickBot="1">
       <c r="B55" s="8"/>
-      <c r="C55" s="17"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" spans="1:7" ht="60.75" thickBot="1">
+    <row r="56" spans="1:7" ht="46" thickBot="1">
       <c r="A56" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="14" t="s">
         <v>512</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -3176,11 +4884,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1">
+    <row r="57" spans="1:7" ht="16" thickBot="1">
       <c r="B57" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="14" t="s">
         <v>513</v>
       </c>
       <c r="D57" s="10" t="s">
@@ -3196,11 +4904,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="60.75" thickBot="1">
+    <row r="58" spans="1:7" ht="61" thickBot="1">
       <c r="B58" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="14" t="s">
         <v>514</v>
       </c>
       <c r="D58" s="10" t="s">
@@ -3216,11 +4924,11 @@
         <v>393</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="45.75" thickBot="1">
+    <row r="59" spans="1:7" ht="31" thickBot="1">
       <c r="B59" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="14" t="s">
         <v>515</v>
       </c>
       <c r="D59" s="10" t="s">
@@ -3236,11 +4944,11 @@
         <v>394</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30.75" thickBot="1">
+    <row r="60" spans="1:7" ht="31" thickBot="1">
       <c r="B60" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="14" t="s">
         <v>299</v>
       </c>
       <c r="D60" s="10" t="s">
@@ -3256,11 +4964,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30.75" thickBot="1">
+    <row r="61" spans="1:7" ht="16" thickBot="1">
       <c r="B61" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="14" t="s">
         <v>516</v>
       </c>
       <c r="D61" s="10" t="s">
@@ -3276,11 +4984,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="45.75" thickBot="1">
+    <row r="62" spans="1:7" ht="46" thickBot="1">
       <c r="B62" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="14" t="s">
         <v>517</v>
       </c>
       <c r="D62" s="10" t="s">
@@ -3296,11 +5004,11 @@
         <v>404</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="60.75" thickBot="1">
+    <row r="63" spans="1:7" ht="46" thickBot="1">
       <c r="B63" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="14" t="s">
         <v>518</v>
       </c>
       <c r="D63" s="10" t="s">
@@ -3316,11 +5024,11 @@
         <v>405</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30.75" thickBot="1">
+    <row r="64" spans="1:7" ht="31" thickBot="1">
       <c r="B64" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="14" t="s">
         <v>519</v>
       </c>
       <c r="D64" s="10" t="s">
@@ -3336,11 +5044,11 @@
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="30.75" thickBot="1">
+    <row r="65" spans="2:7" ht="31" thickBot="1">
       <c r="B65" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="14" t="s">
         <v>520</v>
       </c>
       <c r="D65" s="10" t="s">
@@ -3356,11 +5064,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="45.75" thickBot="1">
+    <row r="66" spans="2:7" ht="46" thickBot="1">
       <c r="B66" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="14" t="s">
         <v>521</v>
       </c>
       <c r="D66" s="10" t="s">
@@ -3376,11 +5084,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="30.75" thickBot="1">
+    <row r="67" spans="2:7" ht="31" thickBot="1">
       <c r="B67" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="14" t="s">
         <v>199</v>
       </c>
       <c r="D67" s="10" t="s">
@@ -3396,11 +5104,11 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="90.75" thickBot="1">
+    <row r="68" spans="2:7" ht="76" thickBot="1">
       <c r="B68" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="14" t="s">
         <v>522</v>
       </c>
       <c r="D68" s="10" t="s">
@@ -3416,11 +5124,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="75.75" thickBot="1">
+    <row r="69" spans="2:7" ht="76" thickBot="1">
       <c r="B69" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C69" s="14" t="s">
         <v>523</v>
       </c>
       <c r="D69" s="10" t="s">
@@ -3436,11 +5144,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="30.75" thickBot="1">
+    <row r="70" spans="2:7" ht="31" thickBot="1">
       <c r="B70" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="14" t="s">
         <v>524</v>
       </c>
       <c r="D70" s="10" t="s">
@@ -3454,11 +5162,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="2:7" ht="75.75" thickBot="1">
+    <row r="71" spans="2:7" ht="76" thickBot="1">
       <c r="B71" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="14" t="s">
         <v>525</v>
       </c>
       <c r="D71" s="10" t="s">
@@ -3478,10 +5186,10 @@
       <c r="B72" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="18" t="s">
+      <c r="C72" s="17" t="s">
         <v>526</v>
       </c>
-      <c r="D72" s="15" t="s">
+      <c r="D72" s="19" t="s">
         <v>482</v>
       </c>
       <c r="E72" s="10" t="s">
@@ -3494,12 +5202,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="2:7" ht="30.75" thickBot="1">
+    <row r="73" spans="2:7" ht="31" thickBot="1">
       <c r="B73" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="15"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="19"/>
       <c r="E73" s="10" t="s">
         <v>203</v>
       </c>
@@ -3510,11 +5218,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="2:7" ht="90.75" thickBot="1">
+    <row r="74" spans="2:7" ht="91" thickBot="1">
       <c r="B74" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C74" s="14" t="s">
         <v>527</v>
       </c>
       <c r="D74" s="10" t="s">
@@ -3530,11 +5238,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="2:7" ht="30.75" thickBot="1">
+    <row r="75" spans="2:7" ht="31" thickBot="1">
       <c r="B75" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="16" t="s">
+      <c r="C75" s="14" t="s">
         <v>528</v>
       </c>
       <c r="D75" s="10" t="s">
@@ -3550,11 +5258,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="2:7" ht="45.75" thickBot="1">
+    <row r="76" spans="2:7" ht="46" thickBot="1">
       <c r="B76" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="C76" s="14" t="s">
         <v>529</v>
       </c>
       <c r="D76" s="10" t="s">
@@ -3570,11 +5278,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="2:7" ht="15.75" thickBot="1">
+    <row r="77" spans="2:7" ht="16" thickBot="1">
       <c r="B77" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="C77" s="14" t="s">
         <v>530</v>
       </c>
       <c r="D77" s="10"/>
@@ -3584,11 +5292,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="2:7" ht="30.75" thickBot="1">
+    <row r="78" spans="2:7" ht="31" thickBot="1">
       <c r="B78" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="14" t="s">
         <v>531</v>
       </c>
       <c r="D78" s="10" t="s">
@@ -3604,11 +5312,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="2:7" ht="45.75" thickBot="1">
+    <row r="79" spans="2:7" ht="31" thickBot="1">
       <c r="B79" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C79" s="14" t="s">
         <v>532</v>
       </c>
       <c r="D79" s="10" t="s">
@@ -3624,11 +5332,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="2:7" ht="45.75" thickBot="1">
+    <row r="80" spans="2:7" ht="46" thickBot="1">
       <c r="B80" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="14" t="s">
         <v>533</v>
       </c>
       <c r="D80" s="10" t="s">
@@ -3644,11 +5352,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="60.75" thickBot="1">
+    <row r="81" spans="1:7" ht="61" thickBot="1">
       <c r="B81" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="C81" s="14" t="s">
         <v>534</v>
       </c>
       <c r="D81" s="10" t="s">
@@ -3664,11 +5372,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="75.75" thickBot="1">
+    <row r="82" spans="1:7" ht="76" thickBot="1">
       <c r="B82" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="C82" s="14" t="s">
         <v>535</v>
       </c>
       <c r="D82" s="10" t="s">
@@ -3684,11 +5392,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.75" thickBot="1">
+    <row r="83" spans="1:7" ht="16" thickBot="1">
       <c r="B83" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C83" s="17"/>
+      <c r="C83" s="15"/>
       <c r="D83" s="10"/>
       <c r="E83" s="10"/>
       <c r="F83" s="10"/>
@@ -3696,11 +5404,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30.75" thickBot="1">
+    <row r="84" spans="1:7" ht="31" thickBot="1">
       <c r="B84" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C84" s="16" t="s">
+      <c r="C84" s="14" t="s">
         <v>536</v>
       </c>
       <c r="D84" s="10" t="s">
@@ -3716,11 +5424,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30.75" thickBot="1">
+    <row r="85" spans="1:7" ht="31" thickBot="1">
       <c r="B85" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="16" t="s">
+      <c r="C85" s="14" t="s">
         <v>537</v>
       </c>
       <c r="D85" s="10" t="s">
@@ -3736,11 +5444,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15.75" thickBot="1">
+    <row r="86" spans="1:7" ht="16" thickBot="1">
       <c r="B86" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C86" s="16" t="s">
+      <c r="C86" s="14" t="s">
         <v>311</v>
       </c>
       <c r="D86" s="10" t="s">
@@ -3756,22 +5464,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15.75" thickBot="1">
+    <row r="87" spans="1:7" ht="16" thickBot="1">
       <c r="B87" s="8"/>
-      <c r="C87" s="17"/>
+      <c r="C87" s="15"/>
       <c r="D87" s="10"/>
       <c r="E87" s="10"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" thickBot="1">
+    <row r="88" spans="1:7" ht="16" thickBot="1">
       <c r="A88" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C88" s="16" t="s">
+      <c r="C88" s="14" t="s">
         <v>538</v>
       </c>
       <c r="D88" s="10" t="s">
@@ -3785,22 +5493,22 @@
       </c>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" thickBot="1">
+    <row r="89" spans="1:7" ht="16" thickBot="1">
       <c r="B89" s="8"/>
-      <c r="C89" s="17"/>
+      <c r="C89" s="15"/>
       <c r="D89" s="10"/>
       <c r="E89" s="10"/>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="1:7" ht="30.75" thickBot="1">
+    <row r="90" spans="1:7" ht="31" thickBot="1">
       <c r="A90" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C90" s="16" t="s">
+      <c r="C90" s="14" t="s">
         <v>539</v>
       </c>
       <c r="D90" s="10" t="s">
@@ -3816,22 +5524,22 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15.75" thickBot="1">
+    <row r="91" spans="1:7" ht="16" thickBot="1">
       <c r="B91" s="8"/>
-      <c r="C91" s="17"/>
+      <c r="C91" s="15"/>
       <c r="D91" s="10"/>
       <c r="E91" s="10"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
     </row>
-    <row r="92" spans="1:7" ht="30.75" thickBot="1">
+    <row r="92" spans="1:7" ht="31" thickBot="1">
       <c r="A92" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="C92" s="14" t="s">
         <v>313</v>
       </c>
       <c r="D92" s="10" t="s">
@@ -3847,22 +5555,22 @@
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15.75" thickBot="1">
+    <row r="93" spans="1:7" ht="16" thickBot="1">
       <c r="B93" s="8"/>
-      <c r="C93" s="17"/>
+      <c r="C93" s="15"/>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75" thickBot="1">
+    <row r="94" spans="1:7" ht="16" thickBot="1">
       <c r="A94" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="C94" s="16" t="s">
+      <c r="C94" s="14" t="s">
         <v>314</v>
       </c>
       <c r="D94" s="10" t="s">
@@ -3878,22 +5586,22 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15.75" thickBot="1">
+    <row r="95" spans="1:7" ht="16" thickBot="1">
       <c r="B95" s="8"/>
-      <c r="C95" s="17"/>
+      <c r="C95" s="15"/>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
     </row>
-    <row r="96" spans="1:7" ht="60.75" thickBot="1">
+    <row r="96" spans="1:7" ht="61" thickBot="1">
       <c r="A96" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C96" s="14" t="s">
         <v>540</v>
       </c>
       <c r="D96" s="10" t="s">
@@ -3909,22 +5617,22 @@
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15.75" thickBot="1">
+    <row r="97" spans="1:7" ht="16" thickBot="1">
       <c r="B97" s="8"/>
-      <c r="C97" s="17"/>
+      <c r="C97" s="15"/>
       <c r="D97" s="10"/>
       <c r="E97" s="10"/>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
     </row>
-    <row r="98" spans="1:7" ht="30.75" thickBot="1">
+    <row r="98" spans="1:7" ht="31" thickBot="1">
       <c r="A98" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="C98" s="16" t="s">
+      <c r="C98" s="14" t="s">
         <v>541</v>
       </c>
       <c r="D98" s="10" t="s">
@@ -3940,22 +5648,22 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15.75" thickBot="1">
+    <row r="99" spans="1:7" ht="16" thickBot="1">
       <c r="B99" s="8"/>
-      <c r="C99" s="17"/>
+      <c r="C99" s="15"/>
       <c r="D99" s="10"/>
       <c r="E99" s="10"/>
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" thickBot="1">
+    <row r="100" spans="1:7" ht="16" thickBot="1">
       <c r="A100" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="C100" s="16" t="s">
+      <c r="C100" s="14" t="s">
         <v>542</v>
       </c>
       <c r="D100" s="10" t="s">
@@ -3971,9 +5679,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15.75" thickBot="1">
+    <row r="101" spans="1:7" ht="16" thickBot="1">
       <c r="B101" s="8"/>
-      <c r="C101" s="17"/>
+      <c r="C101" s="15"/>
       <c r="D101" s="10"/>
       <c r="E101" s="10"/>
       <c r="F101" s="10"/>
@@ -3986,10 +5694,10 @@
       <c r="B102" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="C102" s="18" t="s">
+      <c r="C102" s="17" t="s">
         <v>543</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="D102" s="19" t="s">
         <v>440</v>
       </c>
       <c r="E102" s="10" t="s">
@@ -4002,12 +5710,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="45.75" thickBot="1">
+    <row r="103" spans="1:7" ht="46" thickBot="1">
       <c r="B103" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C103" s="19"/>
-      <c r="D103" s="15"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="19"/>
       <c r="E103" s="10" t="s">
         <v>319</v>
       </c>
@@ -4018,22 +5726,22 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15.75" thickBot="1">
+    <row r="104" spans="1:7" ht="16" thickBot="1">
       <c r="B104" s="8"/>
-      <c r="C104" s="17"/>
+      <c r="C104" s="15"/>
       <c r="D104" s="10"/>
       <c r="E104" s="10"/>
       <c r="F104" s="10"/>
       <c r="G104" s="10"/>
     </row>
-    <row r="105" spans="1:7" ht="30.75" thickBot="1">
+    <row r="105" spans="1:7" ht="16" thickBot="1">
       <c r="A105" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="C105" s="16" t="s">
+      <c r="C105" s="14" t="s">
         <v>320</v>
       </c>
       <c r="D105" s="10" t="s">
@@ -4049,22 +5757,22 @@
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15.75" thickBot="1">
+    <row r="106" spans="1:7" ht="16" thickBot="1">
       <c r="B106" s="8"/>
-      <c r="C106" s="17"/>
+      <c r="C106" s="15"/>
       <c r="D106" s="10"/>
       <c r="E106" s="10"/>
       <c r="F106" s="10"/>
       <c r="G106" s="10"/>
     </row>
-    <row r="107" spans="1:7" ht="30.75" thickBot="1">
+    <row r="107" spans="1:7" ht="31" thickBot="1">
       <c r="A107" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="C107" s="16" t="s">
+      <c r="C107" s="14" t="s">
         <v>321</v>
       </c>
       <c r="D107" s="10" t="s">
@@ -4080,22 +5788,22 @@
         <v>108</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15.75" thickBot="1">
+    <row r="108" spans="1:7" ht="16" thickBot="1">
       <c r="B108" s="8"/>
-      <c r="C108" s="17"/>
+      <c r="C108" s="15"/>
       <c r="D108" s="10"/>
       <c r="E108" s="10"/>
       <c r="F108" s="10"/>
       <c r="G108" s="10"/>
     </row>
-    <row r="109" spans="1:7" ht="45.75" thickBot="1">
+    <row r="109" spans="1:7" ht="46" thickBot="1">
       <c r="A109" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="C109" s="16" t="s">
+      <c r="C109" s="14" t="s">
         <v>544</v>
       </c>
       <c r="D109" s="10" t="s">
@@ -4111,22 +5819,22 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15.75" thickBot="1">
+    <row r="110" spans="1:7" ht="16" thickBot="1">
       <c r="B110" s="8"/>
-      <c r="C110" s="17"/>
+      <c r="C110" s="15"/>
       <c r="D110" s="10"/>
       <c r="E110" s="10"/>
       <c r="F110" s="10"/>
       <c r="G110" s="10"/>
     </row>
-    <row r="111" spans="1:7" ht="45.75" thickBot="1">
+    <row r="111" spans="1:7" ht="46" thickBot="1">
       <c r="A111" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="C111" s="16" t="s">
+      <c r="C111" s="14" t="s">
         <v>545</v>
       </c>
       <c r="D111" s="10" t="s">
@@ -4142,11 +5850,11 @@
         <v>447</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="75.75" thickBot="1">
+    <row r="112" spans="1:7" ht="76" thickBot="1">
       <c r="B112" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="C112" s="16" t="s">
+      <c r="C112" s="14" t="s">
         <v>546</v>
       </c>
       <c r="D112" s="10" t="s">
@@ -4162,11 +5870,11 @@
         <v>448</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="45.75" thickBot="1">
+    <row r="113" spans="1:7" ht="31" thickBot="1">
       <c r="B113" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="16" t="s">
+      <c r="C113" s="14" t="s">
         <v>547</v>
       </c>
       <c r="D113" s="10" t="s">
@@ -4182,11 +5890,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="30.75" thickBot="1">
+    <row r="114" spans="1:7" ht="31" thickBot="1">
       <c r="B114" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C114" s="16" t="s">
+      <c r="C114" s="14" t="s">
         <v>548</v>
       </c>
       <c r="D114" s="10" t="s">
@@ -4202,22 +5910,22 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15.75" thickBot="1">
+    <row r="115" spans="1:7" ht="16" thickBot="1">
       <c r="B115" s="8"/>
-      <c r="C115" s="17"/>
+      <c r="C115" s="15"/>
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
       <c r="G115" s="10"/>
     </row>
-    <row r="116" spans="1:7" ht="30.75" thickBot="1">
+    <row r="116" spans="1:7" ht="31" thickBot="1">
       <c r="A116" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="C116" s="16" t="s">
+      <c r="C116" s="14" t="s">
         <v>549</v>
       </c>
       <c r="D116" s="10" t="s">
@@ -4233,22 +5941,22 @@
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15.75" thickBot="1">
+    <row r="117" spans="1:7" ht="16" thickBot="1">
       <c r="B117" s="8"/>
-      <c r="C117" s="17"/>
+      <c r="C117" s="15"/>
       <c r="D117" s="10"/>
       <c r="E117" s="10"/>
       <c r="F117" s="10"/>
       <c r="G117" s="10"/>
     </row>
-    <row r="118" spans="1:7" ht="45.75" thickBot="1">
+    <row r="118" spans="1:7" ht="46" thickBot="1">
       <c r="A118" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="C118" s="16" t="s">
+      <c r="C118" s="14" t="s">
         <v>550</v>
       </c>
       <c r="D118" s="10" t="s">
@@ -4264,11 +5972,11 @@
         <v>479</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="90.75" thickBot="1">
+    <row r="119" spans="1:7" ht="76" thickBot="1">
       <c r="B119" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C119" s="16" t="s">
+      <c r="C119" s="14" t="s">
         <v>551</v>
       </c>
       <c r="D119" s="10" t="s">
@@ -4284,11 +5992,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="60.75" thickBot="1">
+    <row r="120" spans="1:7" ht="61" thickBot="1">
       <c r="B120" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C120" s="16" t="s">
+      <c r="C120" s="14" t="s">
         <v>552</v>
       </c>
       <c r="D120" s="10" t="s">
@@ -4304,11 +6012,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="45.75" thickBot="1">
+    <row r="121" spans="1:7" ht="46" thickBot="1">
       <c r="B121" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C121" s="16" t="s">
+      <c r="C121" s="14" t="s">
         <v>553</v>
       </c>
       <c r="D121" s="10" t="s">
@@ -4324,11 +6032,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="75.75" thickBot="1">
+    <row r="122" spans="1:7" ht="76" thickBot="1">
       <c r="B122" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="14" t="s">
         <v>554</v>
       </c>
       <c r="D122" s="10" t="s">
@@ -4344,11 +6052,11 @@
         <v>471</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="45.75" thickBot="1">
+    <row r="123" spans="1:7" ht="46" thickBot="1">
       <c r="B123" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="C123" s="16" t="s">
+      <c r="C123" s="14" t="s">
         <v>555</v>
       </c>
       <c r="D123" s="10" t="s">
@@ -4364,11 +6072,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="45.75" thickBot="1">
+    <row r="124" spans="1:7" ht="46" thickBot="1">
       <c r="B124" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C124" s="16" t="s">
+      <c r="C124" s="14" t="s">
         <v>556</v>
       </c>
       <c r="D124" s="10" t="s">
@@ -4384,11 +6092,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="75.75" thickBot="1">
+    <row r="125" spans="1:7" ht="61" thickBot="1">
       <c r="B125" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C125" s="16" t="s">
+      <c r="C125" s="14" t="s">
         <v>557</v>
       </c>
       <c r="D125" s="10" t="s">
@@ -4408,10 +6116,10 @@
       <c r="B126" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C126" s="18" t="s">
+      <c r="C126" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="D126" s="15" t="s">
+      <c r="D126" s="19" t="s">
         <v>460</v>
       </c>
       <c r="E126" s="10" t="s">
@@ -4424,12 +6132,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15.75" thickBot="1">
+    <row r="127" spans="1:7" ht="16" thickBot="1">
       <c r="B127" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C127" s="19"/>
-      <c r="D127" s="15"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="19"/>
       <c r="E127" s="10" t="s">
         <v>333</v>
       </c>
@@ -4444,10 +6152,10 @@
       <c r="B128" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="D128" s="15" t="s">
+      <c r="D128" s="19" t="s">
         <v>461</v>
       </c>
       <c r="E128" s="10" t="s">
@@ -4460,12 +6168,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15.75" thickBot="1">
+    <row r="129" spans="1:7" ht="16" thickBot="1">
       <c r="B129" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C129" s="19"/>
-      <c r="D129" s="15"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="19"/>
       <c r="E129" s="10"/>
       <c r="F129" s="10"/>
       <c r="G129" s="10" t="s">
@@ -4476,10 +6184,10 @@
       <c r="B130" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C130" s="18" t="s">
+      <c r="C130" s="17" t="s">
         <v>560</v>
       </c>
-      <c r="D130" s="15"/>
+      <c r="D130" s="19"/>
       <c r="E130" s="10" t="s">
         <v>244</v>
       </c>
@@ -4490,12 +6198,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="30.75" thickBot="1">
+    <row r="131" spans="1:7" ht="31" thickBot="1">
       <c r="B131" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C131" s="19"/>
-      <c r="D131" s="15"/>
+      <c r="C131" s="18"/>
+      <c r="D131" s="19"/>
       <c r="E131" s="10" t="s">
         <v>243</v>
       </c>
@@ -4506,11 +6214,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="30.75" thickBot="1">
+    <row r="132" spans="1:7" ht="31" thickBot="1">
       <c r="B132" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C132" s="16" t="s">
+      <c r="C132" s="14" t="s">
         <v>335</v>
       </c>
       <c r="D132" s="10" t="s">
@@ -4526,11 +6234,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="30.75" thickBot="1">
+    <row r="133" spans="1:7" ht="31" thickBot="1">
       <c r="B133" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C133" s="16" t="s">
+      <c r="C133" s="14" t="s">
         <v>561</v>
       </c>
       <c r="D133" s="10" t="s">
@@ -4546,11 +6254,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="30.75" thickBot="1">
+    <row r="134" spans="1:7" ht="31" thickBot="1">
       <c r="B134" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C134" s="16" t="s">
+      <c r="C134" s="14" t="s">
         <v>562</v>
       </c>
       <c r="D134" s="10" t="s">
@@ -4566,11 +6274,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="30.75" thickBot="1">
+    <row r="135" spans="1:7" ht="31" thickBot="1">
       <c r="B135" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C135" s="16" t="s">
+      <c r="C135" s="14" t="s">
         <v>563</v>
       </c>
       <c r="D135" s="10" t="s">
@@ -4586,11 +6294,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="45.75" thickBot="1">
+    <row r="136" spans="1:7" ht="31" thickBot="1">
       <c r="B136" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C136" s="16" t="s">
+      <c r="C136" s="14" t="s">
         <v>564</v>
       </c>
       <c r="D136" s="10" t="s">
@@ -4606,11 +6314,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15.75" thickBot="1">
+    <row r="137" spans="1:7" ht="16" thickBot="1">
       <c r="B137" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C137" s="16" t="s">
+      <c r="C137" s="14" t="s">
         <v>340</v>
       </c>
       <c r="D137" s="10" t="s">
@@ -4626,22 +6334,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15.75" thickBot="1">
+    <row r="138" spans="1:7" ht="16" thickBot="1">
       <c r="B138" s="8"/>
-      <c r="C138" s="17"/>
+      <c r="C138" s="15"/>
       <c r="D138" s="10"/>
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
       <c r="G138" s="10"/>
     </row>
-    <row r="139" spans="1:7" ht="15.75" thickBot="1">
+    <row r="139" spans="1:7" ht="16" thickBot="1">
       <c r="A139" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C139" s="16" t="s">
+      <c r="C139" s="14" t="s">
         <v>179</v>
       </c>
       <c r="D139" s="10" t="s">
@@ -4657,22 +6365,22 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15.75" thickBot="1">
+    <row r="140" spans="1:7" ht="16" thickBot="1">
       <c r="B140" s="8"/>
-      <c r="C140" s="17"/>
+      <c r="C140" s="15"/>
       <c r="D140" s="10"/>
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
       <c r="G140" s="10"/>
     </row>
-    <row r="141" spans="1:7" ht="15.75" thickBot="1">
+    <row r="141" spans="1:7" ht="16" thickBot="1">
       <c r="A141" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="C141" s="16" t="s">
+      <c r="C141" s="14" t="s">
         <v>341</v>
       </c>
       <c r="D141" s="10" t="s">
@@ -4688,11 +6396,11 @@
         <v>151</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="30.75" thickBot="1">
+    <row r="142" spans="1:7" ht="31" thickBot="1">
       <c r="B142" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C142" s="16" t="s">
+      <c r="C142" s="14" t="s">
         <v>565</v>
       </c>
       <c r="D142" s="10" t="s">
@@ -4708,11 +6416,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15.75" thickBot="1">
+    <row r="143" spans="1:7" ht="16" thickBot="1">
       <c r="B143" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="17"/>
+      <c r="C143" s="15"/>
       <c r="D143" s="10" t="s">
         <v>467</v>
       </c>
@@ -4726,11 +6434,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="60.75" thickBot="1">
+    <row r="144" spans="1:7" ht="61" thickBot="1">
       <c r="B144" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C144" s="16" t="s">
+      <c r="C144" s="14" t="s">
         <v>566</v>
       </c>
       <c r="D144" s="10" t="s">
@@ -4746,11 +6454,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="2:7" ht="15.75" thickBot="1">
+    <row r="145" spans="2:7" ht="16" thickBot="1">
       <c r="B145" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C145" s="16" t="s">
+      <c r="C145" s="14" t="s">
         <v>344</v>
       </c>
       <c r="D145" s="10" t="s">
@@ -4766,11 +6474,11 @@
         <v>159</v>
       </c>
     </row>
-    <row r="146" spans="2:7" ht="45.75" thickBot="1">
+    <row r="146" spans="2:7" ht="46" thickBot="1">
       <c r="B146" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C146" s="16" t="s">
+      <c r="C146" s="14" t="s">
         <v>567</v>
       </c>
       <c r="D146" s="10" t="s">
@@ -4786,11 +6494,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="147" spans="2:7" ht="15.75" thickBot="1">
+    <row r="147" spans="2:7" ht="16" thickBot="1">
       <c r="B147" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C147" s="16" t="s">
+      <c r="C147" s="14" t="s">
         <v>346</v>
       </c>
       <c r="D147" s="10" t="s">
@@ -4806,11 +6514,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="148" spans="2:7" ht="30.75" thickBot="1">
+    <row r="148" spans="2:7" ht="31" thickBot="1">
       <c r="B148" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C148" s="16" t="s">
+      <c r="C148" s="14" t="s">
         <v>568</v>
       </c>
       <c r="D148" s="10" t="s">
@@ -4834,18 +6542,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="D128:D131"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="D102:D103"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D34:D35"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="E37:E38"/>
     <mergeCell ref="F37:F38"/>
@@ -4858,12 +6554,25 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="D128:D131"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="D102:D103"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="C130:C131"/>
   </mergeCells>
+  <phoneticPr fontId="15"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>